<commit_message>
feat(pipelining): add program for testing basic FPU operations #18
</commit_message>
<xml_diff>
--- a/programs/fpu/fpu-testing-program-basic-operations.xlsx
+++ b/programs/fpu/fpu-testing-program-basic-operations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/vp920_ic_ac_uk/Documents/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\fpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{63B95391-4816-4793-A83F-A9A4D08170A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{678CEC3A-AFC3-4130-AB86-0E5A4B017A1E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D94E6BA-9580-4AC1-BF5D-70CA50A50E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="S9" s="2" t="str">
-        <f t="shared" ref="S9:S23" si="0">DEC2HEX(C9*2^15 + D9*2^14 + E9*2^13 + F9*2^12 + G9*2^11 + H9*2^10 + I9*2^9 + J9*2^8 + K9*2^7 + L9*2^6 + M9*2^5 + N9*2^4 + O9 * 2 ^ 3 + P9  * 2^2 + Q9 * 2 + R9)</f>
+        <f t="shared" ref="S9:S21" si="0">DEC2HEX(C9*2^15 + D9*2^14 + E9*2^13 + F9*2^12 + G9*2^11 + H9*2^10 + I9*2^9 + J9*2^8 + K9*2^7 + L9*2^6 + M9*2^5 + N9*2^4 + O9 * 2 ^ 3 + P9  * 2^2 + Q9 * 2 + R9)</f>
         <v>744</v>
       </c>
     </row>
@@ -1767,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="S22" s="2" t="str">
-        <f>DEC2HEX(C22*2^15 + D22*2^14 + E22*2^13 + F22*2^12 + G22*2^11 + H22*2^10 + I22*2^9 + J22*2^8 + K22*2^7 + L22*2^6 + M22*2^5 + N22*2^4 + O22 * 2 ^ 3 + P22  * 2^2 + Q22 * 2 + R22)</f>
+        <f t="shared" ref="S22:S27" si="2">DEC2HEX(C22*2^15 + D22*2^14 + E22*2^13 + F22*2^12 + G22*2^11 + H22*2^10 + I22*2^9 + J22*2^8 + K22*2^7 + L22*2^6 + M22*2^5 + N22*2^4 + O22 * 2 ^ 3 + P22  * 2^2 + Q22 * 2 + R22)</f>
         <v>D44</v>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="S23" s="2" t="str">
-        <f>DEC2HEX(C23*2^15 + D23*2^14 + E23*2^13 + F23*2^12 + G23*2^11 + H23*2^10 + I23*2^9 + J23*2^8 + K23*2^7 + L23*2^6 + M23*2^5 + N23*2^4 + O23 * 2 ^ 3 + P23  * 2^2 + Q23 * 2 + R23)</f>
+        <f t="shared" si="2"/>
         <v>7000</v>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="S24" s="2" t="str">
-        <f>DEC2HEX(C24*2^15 + D24*2^14 + E24*2^13 + F24*2^12 + G24*2^11 + H24*2^10 + I24*2^9 + J24*2^8 + K24*2^7 + L24*2^6 + M24*2^5 + N24*2^4 + O24 * 2 ^ 3 + P24  * 2^2 + Q24 * 2 + R24)</f>
+        <f t="shared" si="2"/>
         <v>4700</v>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="2" t="str">
-        <f>DEC2HEX(C25*2^15 + D25*2^14 + E25*2^13 + F25*2^12 + G25*2^11 + H25*2^10 + I25*2^9 + J25*2^8 + K25*2^7 + L25*2^6 + M25*2^5 + N25*2^4 + O25 * 2 ^ 3 + P25  * 2^2 + Q25 * 2 + R25)</f>
+        <f t="shared" si="2"/>
         <v>4600</v>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
         <v>0</v>
       </c>
       <c r="S26" s="2" t="str">
-        <f>DEC2HEX(C26*2^15 + D26*2^14 + E26*2^13 + F26*2^12 + G26*2^11 + H26*2^10 + I26*2^9 + J26*2^8 + K26*2^7 + L26*2^6 + M26*2^5 + N26*2^4 + O26 * 2 ^ 3 + P26  * 2^2 + Q26 * 2 + R26)</f>
+        <f t="shared" si="2"/>
         <v>4A80</v>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="S27" s="2" t="str">
-        <f>DEC2HEX(C27*2^15 + D27*2^14 + E27*2^13 + F27*2^12 + G27*2^11 + H27*2^10 + I27*2^9 + J27*2^8 + K27*2^7 + L27*2^6 + M27*2^5 + N27*2^4 + O27 * 2 ^ 3 + P27  * 2^2 + Q27 * 2 + R27)</f>
+        <f t="shared" si="2"/>
         <v>3C00</v>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
         <v>0</v>
       </c>
       <c r="S28" s="2" t="str">
-        <f t="shared" ref="S28:S29" si="2">DEC2HEX(C28*2^15 + D28*2^14 + E28*2^13 + F28*2^12 + G28*2^11 + H28*2^10 + I28*2^9 + J28*2^8 + K28*2^7 + L28*2^6 + M28*2^5 + N28*2^4 + O28 * 2 ^ 3 + P28  * 2^2 + Q28 * 2 + R28)</f>
+        <f t="shared" ref="S28:S29" si="3">DEC2HEX(C28*2^15 + D28*2^14 + E28*2^13 + F28*2^12 + G28*2^11 + H28*2^10 + I28*2^9 + J28*2^8 + K28*2^7 + L28*2^6 + M28*2^5 + N28*2^4 + O28 * 2 ^ 3 + P28  * 2^2 + Q28 * 2 + R28)</f>
         <v>BC00</v>
       </c>
     </row>
@@ -2187,12 +2187,22 @@
         <v>0</v>
       </c>
       <c r="S29" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5140</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="K6:P6"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="K2:M2"/>
@@ -2202,16 +2212,6 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:R5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>